<commit_message>
merge data with dem
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,80 +440,155 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PAT_ENC_CSN_ID</t>
+          <t>Hospital</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Amoxicillin</t>
+          <t>CSN</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Patient</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SEX_NAME</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Age_At_Admission</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DAYS_TO_READMISSION</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Mortality from Index Culture (Days)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>LOS_Days</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Admission Date</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Discharge Date</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ICU_Encounter</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Culture</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Index_Culture</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Polymicrobial_Infection</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Patient_Had_ID_consult</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Diagnosis_Endocarditis_This_Encounter</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Diagnosis_Osteomyelitis_This_Encounter</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>Cefepime</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Piperacillin/Tazobactam</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Group</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Total_DOT</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Last_Admin</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="n">
         <v>8</v>
       </c>
-      <c r="D2" t="n">
+      <c r="T2" t="n">
         <v>7</v>
       </c>
-      <c r="E2" t="n">
+      <c r="U2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="n">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>44598.28888888889</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>44592</v>
+      <c r="V2" t="n">
+        <v>12</v>
+      </c>
+      <c r="W2" s="2" t="n">
+        <v>44598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>